<commit_message>
[expression] - fix code to support negative number parsing
[csv]
- [`compareExtended`]: fix code to support negative number parsing

[web]
- [closeAll`]: A **NEW** System variable [`nexial.browser.electron.forceTerminate`] to forcefully terminate the AUT executable - i.e. the electron application as specified via [`nexial.browser.electron.appLocation` - after the underlying chromedriver shuts down or when [web >> `closeAll`] is invoked.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_buildnum.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_buildnum.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C9DF54-D1E3-A24A-A9ED-88E99F47D155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5394BB8C-8E80-6141-B17F-EC940892D70B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="-7040" windowWidth="38400" windowHeight="7040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="-7040" windowWidth="38400" windowHeight="7040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -38,10 +38,18 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -752,7 +760,7 @@
   <dimension ref="A1:AAA200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>

</xml_diff>